<commit_message>
Spelling error corrected & style simplified
</commit_message>
<xml_diff>
--- a/examples/game_tables/table.xlsx
+++ b/examples/game_tables/table.xlsx
@@ -7,7 +7,9 @@
     <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="10035"/>
   </bookViews>
   <sheets>
-    <sheet name="table" sheetId="1" r:id="rId1"/>
+    <sheet name="Table" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -15,7 +17,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -26,42 +28,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="4"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="5"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="6"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="7"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="1"/>
       <scheme val="major"/>
@@ -70,16 +37,7 @@
       <b/>
       <i/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <family val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="1"/>
       <scheme val="major"/>
@@ -87,72 +45,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="1"/>
-      <scheme val="major"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -167,64 +70,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,163 +398,163 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+      <c r="A1" s="6">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="6">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="6">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="6">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1" s="6">
         <f>1</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="str">
+      <c r="A2" s="1" t="str">
         <f>"sheet"</f>
         <v>sheet</v>
       </c>
-      <c r="B2" s="9" t="str">
+      <c r="B2" s="1" t="str">
         <f>"ice"</f>
         <v>ice</v>
       </c>
-      <c r="C2" s="10" t="str">
+      <c r="C2" s="1" t="str">
         <f>"Mary"</f>
         <v>Mary</v>
       </c>
-      <c r="D2" s="11" t="str">
+      <c r="D2" s="1" t="str">
         <f>"Google Drive"</f>
         <v>Google Drive</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="str">
+      <c r="A3" s="1" t="str">
         <f>"cellulose"</f>
         <v>cellulose</v>
       </c>
-      <c r="B3" s="9" t="str">
+      <c r="B3" s="1" t="str">
         <f>"Christmas"</f>
         <v>Christmas</v>
       </c>
-      <c r="C3" s="10" t="str">
+      <c r="C3" s="1" t="str">
         <f>"had"</f>
         <v>had</v>
       </c>
-      <c r="D3" s="11" t="str">
+      <c r="D3" s="1" t="str">
         <f>"storm"</f>
         <v>storm</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="str">
+      <c r="A4" s="1" t="str">
         <f>"academia"</f>
         <v>academia</v>
       </c>
-      <c r="B4" s="9" t="str">
+      <c r="B4" s="1" t="str">
         <f>"flake"</f>
         <v>flake</v>
       </c>
-      <c r="C4" s="10" t="str">
+      <c r="C4" s="1" t="str">
         <f>"a"</f>
         <v>a</v>
       </c>
-      <c r="D4" s="11" t="str">
+      <c r="D4" s="1" t="str">
         <f>"sky"</f>
         <v>sky</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="str">
+      <c r="A5" s="1" t="str">
         <f>"printer"</f>
         <v>printer</v>
       </c>
-      <c r="B5" s="9" t="str">
+      <c r="B5" s="1" t="str">
         <f>"mountain top"</f>
         <v>mountain top</v>
       </c>
-      <c r="C5" s="10" t="str">
+      <c r="C5" s="1" t="str">
         <f>"little"</f>
         <v>little</v>
       </c>
-      <c r="D5" s="11" t="str">
+      <c r="D5" s="1" t="str">
         <f>"water"</f>
         <v>water</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="str">
+      <c r="A6" s="4" t="str">
         <f>"paper"</f>
         <v>paper</v>
       </c>
-      <c r="B6" s="14" t="str">
+      <c r="B6" s="4" t="str">
         <f>"snow"</f>
         <v>snow</v>
       </c>
-      <c r="C6" s="16" t="str">
+      <c r="C6" s="4" t="str">
         <f>"lamb"</f>
         <v>lamb</v>
       </c>
-      <c r="D6" s="18" t="str">
+      <c r="D6" s="4" t="str">
         <f>"cloud"</f>
         <v>cloud</v>
       </c>
-      <c r="E6" s="7" t="str">
+      <c r="E6" s="5" t="str">
         <f>"white"</f>
         <v>white</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="str">
+      <c r="A7" s="2" t="str">
         <f>"papers"</f>
         <v>papers</v>
       </c>
-      <c r="B7" s="15" t="str">
+      <c r="B7" s="2" t="str">
         <f>"snowy"</f>
         <v>snowy</v>
       </c>
-      <c r="C7" s="17" t="str">
+      <c r="C7" s="2" t="str">
         <f>"sheep"</f>
         <v>sheep</v>
       </c>
-      <c r="D7" s="19" t="str">
+      <c r="D7" s="2" t="str">
         <f>"clouds"</f>
         <v>clouds</v>
       </c>
-      <c r="E7" s="6" t="str">
+      <c r="E7" s="3" t="str">
         <f>"white colour"</f>
         <v>white colour</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="str">
+      <c r="B8" s="2" t="str">
         <f>"snowing"</f>
         <v>snowing</v>
       </c>
-      <c r="C8" s="17" t="str">
+      <c r="C8" s="2" t="str">
         <f>"Aries"</f>
         <v>Aries</v>
       </c>
-      <c r="D8" s="19" t="str">
-        <f>"clowdy"</f>
-        <v>clowdy</v>
-      </c>
-      <c r="E8" s="6" t="str">
+      <c r="D8" s="2" t="str">
+        <f>"cloudy"</f>
+        <v>cloudy</v>
+      </c>
+      <c r="E8" s="3" t="str">
         <f>"white color"</f>
         <v>white color</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E9" s="6" t="str">
+      <c r="E9" s="3" t="str">
         <f>"whiteness"</f>
         <v>whiteness</v>
       </c>
@@ -699,4 +563,28 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>